<commit_message>
Plus de crash, manque demande permission
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="Sprint 3 Pierre-Luc" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3088,7 +3087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -3914,8 +3913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Backlog et notif aux 60s
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\ESP\Projet-ESP-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Projet\Projet-ESP-\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="9" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="160">
   <si>
     <t>ID</t>
   </si>
@@ -328,9 +328,6 @@
     <t>En tant qu'utilisateur, je veux avoir access aux information de la base de donnée sur iOS, afin de pouvoir utiliser l'application sur iPhone</t>
   </si>
   <si>
-    <t>installer les dépendaces pour compatibilité firebase firestore sur iOS</t>
-  </si>
-  <si>
     <t>La communication entre l'application et la base de donnée doit être possible sur iOS</t>
   </si>
   <si>
@@ -352,9 +349,6 @@
     <t>En tant qu'utilisateur je souhaite avoir des notification lorsque je suis proche d'une sculpture sur iOS, afin de rendre mon expérience sur iOS la même que sur android</t>
   </si>
   <si>
-    <t>Rendre l'application et la feature de notification possible sur ios</t>
-  </si>
-  <si>
     <t>En tant que programmeur, je souhaite que mes données ne soit chargee qu'une seul fois afin de limiter le trafic internet et le nombre de lecture à la base de donnée</t>
   </si>
   <si>
@@ -467,6 +461,60 @@
   </si>
   <si>
     <t>Lorsque l'utilisateur appuie sur une sculpture, l'écran des détails s'ouvrent</t>
+  </si>
+  <si>
+    <t>On doit recevoir une notification lorsqu'on est dans un rayon de 25 m comme sur android</t>
+  </si>
+  <si>
+    <t>Les dépendaces pour compatibilité firebase firestore sur iOS doivent fonctionner</t>
+  </si>
+  <si>
+    <t>On doit pouvoir recevoir une notification même lorsque l'app est en background</t>
+  </si>
+  <si>
+    <t>En tant qu'administrateur, je veux pouvoir ajouter des collaboratuers afin de mettre à jour la liste des collaborateurs</t>
+  </si>
+  <si>
+    <t>Dans l'app admin, un onglet Ajouter des collaborateurs sera présent</t>
+  </si>
+  <si>
+    <t>Champs: Nom et rôle</t>
+  </si>
+  <si>
+    <t>Cliquer sur enregistrer pour confirmer l'envoie du collaborateur</t>
+  </si>
+  <si>
+    <t>Cliquer sur annuler pour interrompre l'ajout du collaborateur</t>
+  </si>
+  <si>
+    <t>En tant qu'administrateur, je veux pouvoir modifier un collaborateur afin de corriger des erreures commisent lors de la création</t>
+  </si>
+  <si>
+    <t>Avoir une liste des collaborateurs déjà dans la base de donnée</t>
+  </si>
+  <si>
+    <t>Pouvoir cliquer sur un collaborateur pour pouvoir le modifier</t>
+  </si>
+  <si>
+    <t>Avoir les champs disponible dans l'objets (nom, rôle)</t>
+  </si>
+  <si>
+    <t>Il devra avoir un icon dans le detail des sculpture pour ouvrir l'application en question</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je souhaite avoir un icone pour l'application afin de pouvoir la distinguer des autres applications sur iOS</t>
+  </si>
+  <si>
+    <t>L'icone doit être le logo de Beauce Art</t>
+  </si>
+  <si>
+    <t>La notification doit avertir l'utilisateur que'il est proche d'une sculpture</t>
+  </si>
+  <si>
+    <t>Lorsque la notification est appuyée, l'application doit s'ouvrir si elle est fermé</t>
+  </si>
+  <si>
+    <t>Lorsque la notification est appuyée, on doit faire un zoom sur la position de l'utilisateur si il est toujours dans un rayon de 25m d'une sculpture</t>
   </si>
 </sst>
 </file>
@@ -558,7 +606,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -625,30 +673,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -657,7 +681,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
@@ -680,8 +704,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1007,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F136" sqref="F136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,146 +1663,146 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="22">
+      <c r="A47" s="20">
         <v>11</v>
       </c>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23">
-        <v>5</v>
-      </c>
-      <c r="D47" s="23">
+      <c r="B47" s="21"/>
+      <c r="C47" s="21">
+        <v>5</v>
+      </c>
+      <c r="D47" s="21">
         <v>40</v>
       </c>
-      <c r="E47" s="23">
+      <c r="E47" s="21">
         <v>11</v>
       </c>
-      <c r="F47" s="24" t="s">
+      <c r="F47" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
-      <c r="B48" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="28" t="s">
+      <c r="A48" s="23"/>
+      <c r="B48" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="28" t="s">
+      <c r="A49" s="23"/>
+      <c r="B49" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="26" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
-      <c r="B50" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="28" t="s">
+      <c r="A50" s="23"/>
+      <c r="B50" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="26" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="22">
+      <c r="A51" s="20">
         <v>12</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23">
-        <v>5</v>
-      </c>
-      <c r="D51" s="23">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21">
+        <v>5</v>
+      </c>
+      <c r="D51" s="21">
         <v>35</v>
       </c>
-      <c r="E51" s="23">
+      <c r="E51" s="21">
         <v>12</v>
       </c>
-      <c r="F51" s="24" t="s">
+      <c r="F51" s="22" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
-      <c r="B52" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="28" t="s">
+      <c r="A52" s="23"/>
+      <c r="B52" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="26" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
-      <c r="B53" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="28" t="s">
+      <c r="A53" s="23"/>
+      <c r="B53" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="25"/>
-      <c r="B54" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="28" t="s">
+      <c r="A54" s="23"/>
+      <c r="B54" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
-      <c r="B55" s="26" t="s">
+      <c r="A55" s="23"/>
+      <c r="B55" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="28" t="s">
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="25"/>
-      <c r="B56" s="26" t="s">
+      <c r="A56" s="23"/>
+      <c r="B56" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="28" t="s">
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="26" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
-      <c r="B57" s="26" t="s">
+      <c r="A57" s="23"/>
+      <c r="B57" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="28" t="s">
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2027,7 +2049,7 @@
         <v>19</v>
       </c>
       <c r="F74" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2039,7 +2061,7 @@
       <c r="D75" s="18"/>
       <c r="E75" s="18"/>
       <c r="F75" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2051,7 +2073,7 @@
       <c r="D76" s="18"/>
       <c r="E76" s="18"/>
       <c r="F76" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2063,7 +2085,7 @@
       <c r="D77" s="18"/>
       <c r="E77" s="18"/>
       <c r="F77" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2081,7 +2103,7 @@
         <v>20</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2093,7 +2115,7 @@
       <c r="D79" s="18"/>
       <c r="E79" s="18"/>
       <c r="F79" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2105,7 +2127,7 @@
       <c r="D80" s="18"/>
       <c r="E80" s="18"/>
       <c r="F80" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2122,8 +2144,8 @@
       <c r="E81" s="13">
         <v>21</v>
       </c>
-      <c r="F81" s="29" t="s">
-        <v>115</v>
+      <c r="F81" s="27" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2135,7 +2157,7 @@
       <c r="D82" s="18"/>
       <c r="E82" s="17"/>
       <c r="F82" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2147,7 +2169,7 @@
       <c r="D83" s="18"/>
       <c r="E83" s="17"/>
       <c r="F83" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2159,7 +2181,7 @@
       <c r="D84" s="18"/>
       <c r="E84" s="17"/>
       <c r="F84" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2171,7 +2193,7 @@
       <c r="D85" s="18"/>
       <c r="E85" s="17"/>
       <c r="F85" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2183,7 +2205,7 @@
       <c r="D86" s="18"/>
       <c r="E86" s="17"/>
       <c r="F86" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2195,19 +2217,19 @@
       <c r="D87" s="18"/>
       <c r="E87" s="17"/>
       <c r="F87" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="17"/>
       <c r="B88" s="19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C88" s="18"/>
       <c r="D88" s="18"/>
       <c r="E88" s="17"/>
       <c r="F88" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2219,13 +2241,13 @@
         <v>8</v>
       </c>
       <c r="D89" s="14">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E89" s="13">
         <v>22</v>
       </c>
-      <c r="F89" s="29" t="s">
-        <v>122</v>
+      <c r="F89" s="27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2236,8 +2258,8 @@
       <c r="C90" s="18"/>
       <c r="D90" s="18"/>
       <c r="E90" s="17"/>
-      <c r="F90" s="9" t="s">
-        <v>123</v>
+      <c r="F90" s="57" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2248,8 +2270,8 @@
       <c r="C91" s="18"/>
       <c r="D91" s="18"/>
       <c r="E91" s="17"/>
-      <c r="F91" s="9" t="s">
-        <v>124</v>
+      <c r="F91" s="57" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2260,8 +2282,8 @@
       <c r="C92" s="18"/>
       <c r="D92" s="18"/>
       <c r="E92" s="17"/>
-      <c r="F92" s="9" t="s">
-        <v>125</v>
+      <c r="F92" s="57" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2272,8 +2294,8 @@
       <c r="C93" s="18"/>
       <c r="D93" s="18"/>
       <c r="E93" s="17"/>
-      <c r="F93" s="9" t="s">
-        <v>126</v>
+      <c r="F93" s="57" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2284,8 +2306,8 @@
       <c r="C94" s="18"/>
       <c r="D94" s="18"/>
       <c r="E94" s="17"/>
-      <c r="F94" s="9" t="s">
-        <v>127</v>
+      <c r="F94" s="57" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2296,8 +2318,8 @@
       <c r="C95" s="18"/>
       <c r="D95" s="18"/>
       <c r="E95" s="17"/>
-      <c r="F95" s="9" t="s">
-        <v>128</v>
+      <c r="F95" s="57" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2309,13 +2331,13 @@
         <v>5</v>
       </c>
       <c r="D96" s="14">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E96" s="13">
         <v>23</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2326,8 +2348,8 @@
       <c r="C97" s="18"/>
       <c r="D97" s="18"/>
       <c r="E97" s="17"/>
-      <c r="F97" s="9" t="s">
-        <v>130</v>
+      <c r="F97" s="57" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2338,8 +2360,8 @@
       <c r="C98" s="18"/>
       <c r="D98" s="18"/>
       <c r="E98" s="17"/>
-      <c r="F98" s="9" t="s">
-        <v>131</v>
+      <c r="F98" s="57" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2350,8 +2372,8 @@
       <c r="C99" s="18"/>
       <c r="D99" s="18"/>
       <c r="E99" s="17"/>
-      <c r="F99" s="9" t="s">
-        <v>132</v>
+      <c r="F99" s="57" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2368,8 +2390,8 @@
       <c r="E100" s="13">
         <v>24</v>
       </c>
-      <c r="F100" s="29" t="s">
-        <v>133</v>
+      <c r="F100" s="27" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2381,7 +2403,7 @@
       <c r="D101" s="18"/>
       <c r="E101" s="17"/>
       <c r="F101" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2393,7 +2415,7 @@
       <c r="D102" s="18"/>
       <c r="E102" s="17"/>
       <c r="F102" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2405,7 +2427,7 @@
       <c r="D103" s="18"/>
       <c r="E103" s="17"/>
       <c r="F103" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2417,7 +2439,7 @@
       <c r="D104" s="18"/>
       <c r="E104" s="17"/>
       <c r="F104" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -2429,7 +2451,7 @@
       <c r="D105" s="18"/>
       <c r="E105" s="17"/>
       <c r="F105" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -2537,7 +2559,7 @@
       <c r="D113" s="18"/>
       <c r="E113" s="18"/>
       <c r="F113" s="10" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2567,7 +2589,7 @@
         <v>27</v>
       </c>
       <c r="F115" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -2643,7 +2665,7 @@
       <c r="B121" s="14"/>
       <c r="C121" s="14"/>
       <c r="D121" s="14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E121" s="14">
         <v>29</v>
@@ -2660,8 +2682,8 @@
       <c r="C122" s="18"/>
       <c r="D122" s="18"/>
       <c r="E122" s="18"/>
-      <c r="F122" s="10" t="s">
-        <v>97</v>
+      <c r="F122" s="58" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -2672,8 +2694,8 @@
       <c r="C123" s="18"/>
       <c r="D123" s="18"/>
       <c r="E123" s="18"/>
-      <c r="F123" s="10" t="s">
-        <v>98</v>
+      <c r="F123" s="58" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -2691,7 +2713,7 @@
         <v>30</v>
       </c>
       <c r="F124" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -2703,7 +2725,7 @@
       <c r="D125" s="18"/>
       <c r="E125" s="18"/>
       <c r="F125" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -2719,7 +2741,7 @@
         <v>31</v>
       </c>
       <c r="F126" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -2731,7 +2753,7 @@
       <c r="D127" s="18"/>
       <c r="E127" s="18"/>
       <c r="F127" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -2755,7 +2777,7 @@
       <c r="D129" s="18"/>
       <c r="E129" s="18"/>
       <c r="F129" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -2767,42 +2789,303 @@
         <v>8</v>
       </c>
       <c r="D130" s="14">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E130" s="14">
         <v>32</v>
       </c>
       <c r="F130" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="20"/>
-      <c r="B131" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C131" s="21"/>
-      <c r="D131" s="21"/>
-      <c r="E131" s="21"/>
-      <c r="F131" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="11"/>
-      <c r="B132" s="11"/>
-      <c r="C132" s="11">
-        <f>SUM(C2:C131)</f>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="17"/>
+      <c r="B131" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131" s="18"/>
+      <c r="D131" s="18"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="58" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="17"/>
+      <c r="B132" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132" s="18"/>
+      <c r="D132" s="18"/>
+      <c r="E132" s="18"/>
+      <c r="F132" s="58" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="17"/>
+      <c r="B133" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C133" s="18"/>
+      <c r="D133" s="18"/>
+      <c r="E133" s="18"/>
+      <c r="F133" s="58" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="17"/>
+      <c r="B134" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" s="18"/>
+      <c r="D134" s="18"/>
+      <c r="E134" s="18"/>
+      <c r="F134" s="58" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="17"/>
+      <c r="B135" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" s="18"/>
+      <c r="D135" s="18"/>
+      <c r="E135" s="18"/>
+      <c r="F135" s="58" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="13">
+        <v>33</v>
+      </c>
+      <c r="B136" s="14"/>
+      <c r="C136" s="14">
+        <v>8</v>
+      </c>
+      <c r="D136" s="14">
+        <v>20</v>
+      </c>
+      <c r="E136" s="13">
+        <v>33</v>
+      </c>
+      <c r="F136" s="27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="17"/>
+      <c r="B137" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137" s="18"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="17"/>
+      <c r="B138" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C138" s="18"/>
+      <c r="D138" s="18"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="17"/>
+      <c r="B139" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C139" s="18"/>
+      <c r="D139" s="18"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="57" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="17"/>
+      <c r="B140" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" s="18"/>
+      <c r="D140" s="18"/>
+      <c r="E140" s="17"/>
+      <c r="F140" s="57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="17"/>
+      <c r="B141" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" s="18"/>
+      <c r="D141" s="18"/>
+      <c r="E141" s="17"/>
+      <c r="F141" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="D132" s="11">
-        <f>SUM(D2:D131)</f>
-        <v>905</v>
-      </c>
-      <c r="E132" s="11"/>
-      <c r="F132" s="11"/>
-    </row>
-    <row r="133" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="13">
+        <v>34</v>
+      </c>
+      <c r="B142" s="14"/>
+      <c r="C142" s="14">
+        <v>5</v>
+      </c>
+      <c r="D142" s="14">
+        <v>25</v>
+      </c>
+      <c r="E142" s="13">
+        <v>34</v>
+      </c>
+      <c r="F142" s="14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="17"/>
+      <c r="B143" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143" s="18"/>
+      <c r="D143" s="18"/>
+      <c r="E143" s="17"/>
+      <c r="F143" s="57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="17"/>
+      <c r="B144" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144" s="18"/>
+      <c r="D144" s="18"/>
+      <c r="E144" s="17"/>
+      <c r="F144" s="57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="17"/>
+      <c r="B145" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C145" s="18"/>
+      <c r="D145" s="18"/>
+      <c r="E145" s="17"/>
+      <c r="F145" s="57" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="16">
+        <v>35</v>
+      </c>
+      <c r="B146" s="12"/>
+      <c r="C146" s="16"/>
+      <c r="D146" s="16">
+        <v>5</v>
+      </c>
+      <c r="E146" s="16">
+        <v>35</v>
+      </c>
+      <c r="F146" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="54"/>
+      <c r="B147" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" s="54"/>
+      <c r="D147" s="54"/>
+      <c r="E147" s="54"/>
+      <c r="F147" s="58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="54"/>
+      <c r="B148" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148" s="54"/>
+      <c r="D148" s="54"/>
+      <c r="E148" s="54"/>
+      <c r="F148" s="58" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="54"/>
+      <c r="B149" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C149" s="54"/>
+      <c r="D149" s="54"/>
+      <c r="E149" s="54"/>
+      <c r="F149" s="58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="16">
+        <v>36</v>
+      </c>
+      <c r="B150" s="12"/>
+      <c r="C150" s="16"/>
+      <c r="D150" s="16">
+        <v>5</v>
+      </c>
+      <c r="E150" s="16">
+        <v>36</v>
+      </c>
+      <c r="F150" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="54"/>
+      <c r="B151" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151" s="54"/>
+      <c r="D151" s="54"/>
+      <c r="E151" s="54"/>
+      <c r="F151" s="58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="155" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="11"/>
+      <c r="B155" s="11"/>
+      <c r="C155" s="11">
+        <f>SUM(C2:C129)</f>
+        <v>141</v>
+      </c>
+      <c r="D155" s="11">
+        <f>SUM(D2:D129)</f>
+        <v>870</v>
+      </c>
+      <c r="E155" s="11"/>
+      <c r="F155" s="11"/>
+    </row>
+    <row r="156" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2810,10 +3093,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2822,22 +3105,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="49" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2867,7 +3150,7 @@
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="58" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2879,7 +3162,7 @@
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="58" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2891,7 +3174,7 @@
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
-      <c r="F5" s="60" t="s">
+      <c r="F5" s="58" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2908,7 +3191,7 @@
         <v>31</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2919,8 +3202,8 @@
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="60" t="s">
-        <v>102</v>
+      <c r="F7" s="58" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2931,7 +3214,7 @@
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="58" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2943,8 +3226,88 @@
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
-      <c r="F9" s="60" t="s">
-        <v>103</v>
+      <c r="F9" s="58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>35</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16">
+        <v>5</v>
+      </c>
+      <c r="E10" s="16">
+        <v>35</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="54"/>
+      <c r="B11" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="54"/>
+      <c r="B12" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="58" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="54"/>
+      <c r="B13" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>36</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16">
+        <v>5</v>
+      </c>
+      <c r="E14" s="16">
+        <v>36</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="B15" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="58" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2954,10 +3317,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,22 +3329,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="49" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2992,7 +3355,7 @@
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E2" s="14">
         <v>29</v>
@@ -3009,8 +3372,8 @@
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
-      <c r="F3" s="60" t="s">
-        <v>97</v>
+      <c r="F3" s="58" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3021,8 +3384,8 @@
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
-      <c r="F4" s="60" t="s">
-        <v>98</v>
+      <c r="F4" s="58" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3034,28 +3397,75 @@
         <v>8</v>
       </c>
       <c r="D5" s="14">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E5" s="14">
         <v>32</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="60" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="58" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="58" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="58" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="58" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="58" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3063,10 +3473,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A10:F21"/>
+  <dimension ref="A10:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:F21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3075,22 +3485,22 @@
   </cols>
   <sheetData>
     <row r="10" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="51" t="s">
+      <c r="F10" s="49" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3103,13 +3513,13 @@
         <v>8</v>
       </c>
       <c r="D11" s="14">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E11" s="13">
         <v>22</v>
       </c>
-      <c r="F11" s="29" t="s">
-        <v>122</v>
+      <c r="F11" s="27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3120,8 +3530,8 @@
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="17"/>
-      <c r="F12" s="59" t="s">
-        <v>123</v>
+      <c r="F12" s="57" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3132,8 +3542,8 @@
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17"/>
-      <c r="F13" s="59" t="s">
-        <v>124</v>
+      <c r="F13" s="57" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3144,8 +3554,8 @@
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="17"/>
-      <c r="F14" s="59" t="s">
-        <v>125</v>
+      <c r="F14" s="57" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3156,8 +3566,8 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="17"/>
-      <c r="F15" s="59" t="s">
-        <v>126</v>
+      <c r="F15" s="57" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3168,8 +3578,8 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="59" t="s">
-        <v>127</v>
+      <c r="F16" s="57" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3180,8 +3590,8 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="17"/>
-      <c r="F17" s="59" t="s">
-        <v>128</v>
+      <c r="F17" s="57" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3193,13 +3603,13 @@
         <v>5</v>
       </c>
       <c r="D18" s="14">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E18" s="13">
         <v>23</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3210,8 +3620,8 @@
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="17"/>
-      <c r="F19" s="59" t="s">
-        <v>130</v>
+      <c r="F19" s="57" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3222,8 +3632,8 @@
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="17"/>
-      <c r="F20" s="59" t="s">
-        <v>131</v>
+      <c r="F20" s="57" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3234,8 +3644,140 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="17"/>
-      <c r="F21" s="59" t="s">
-        <v>132</v>
+      <c r="F21" s="57" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>33</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14">
+        <v>8</v>
+      </c>
+      <c r="D22" s="14">
+        <v>20</v>
+      </c>
+      <c r="E22" s="13">
+        <v>33</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="57" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>34</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14">
+        <v>5</v>
+      </c>
+      <c r="D28" s="14">
+        <v>25</v>
+      </c>
+      <c r="E28" s="13">
+        <v>34</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="57" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3621,57 +4163,57 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30">
-        <v>8</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31">
+      <c r="A7" s="28">
+        <v>8</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29">
         <v>3</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="29">
         <v>45</v>
       </c>
-      <c r="E7" s="31">
-        <v>8</v>
-      </c>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="29">
+        <v>8</v>
+      </c>
+      <c r="F7" s="32" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36" t="s">
-        <v>140</v>
+      <c r="A8" s="30"/>
+      <c r="B8" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="34" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="34" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="36" t="s">
-        <v>141</v>
+      <c r="A10" s="30"/>
+      <c r="B10" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="34" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3693,76 +4235,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="49" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="54">
+      <c r="A2" s="52">
         <v>10</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53">
         <v>3</v>
       </c>
-      <c r="D2" s="55">
+      <c r="D2" s="53">
         <v>25</v>
       </c>
-      <c r="E2" s="55">
+      <c r="E2" s="53">
         <v>10</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="56" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="60" t="s">
+      <c r="A3" s="54"/>
+      <c r="B3" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="58" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="60" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="58" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="60" t="s">
+      <c r="A5" s="54"/>
+      <c r="B5" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="58" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3883,69 +4425,69 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
+      <c r="A8" s="35">
         <v>9</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38">
+      <c r="B8" s="36"/>
+      <c r="C8" s="36">
         <v>3</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="36">
         <v>25</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="36">
         <v>9</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="39" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="43" t="s">
-        <v>142</v>
+      <c r="A9" s="37"/>
+      <c r="B9" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="41" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="43" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="41" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="43" t="s">
+      <c r="A11" s="37"/>
+      <c r="B11" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="41" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="42" t="s">
+      <c r="A12" s="37"/>
+      <c r="B12" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="43" t="s">
-        <v>143</v>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="41" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4041,32 +4583,32 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="44">
+      <c r="A6" s="42">
         <v>14</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43">
         <v>3</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="43">
         <v>25</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="43">
         <v>14</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="46" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="50" t="s">
+      <c r="A7" s="44"/>
+      <c r="B7" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="48" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4080,7 +4622,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4176,8 +4718,8 @@
       <c r="E6" s="13">
         <v>21</v>
       </c>
-      <c r="F6" s="29" t="s">
-        <v>115</v>
+      <c r="F6" s="27" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4189,7 +4731,7 @@
       <c r="D7" s="18"/>
       <c r="E7" s="17"/>
       <c r="F7" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4201,7 +4743,7 @@
       <c r="D8" s="18"/>
       <c r="E8" s="17"/>
       <c r="F8" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4213,7 +4755,7 @@
       <c r="D9" s="18"/>
       <c r="E9" s="17"/>
       <c r="F9" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4225,7 +4767,7 @@
       <c r="D10" s="18"/>
       <c r="E10" s="17"/>
       <c r="F10" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4237,7 +4779,7 @@
       <c r="D11" s="18"/>
       <c r="E11" s="17"/>
       <c r="F11" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4249,19 +4791,19 @@
       <c r="D12" s="18"/>
       <c r="E12" s="17"/>
       <c r="F12" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17"/>
       <c r="F13" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4278,8 +4820,8 @@
       <c r="E14" s="13">
         <v>24</v>
       </c>
-      <c r="F14" s="29" t="s">
-        <v>133</v>
+      <c r="F14" s="27" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4291,7 +4833,7 @@
       <c r="D15" s="18"/>
       <c r="E15" s="17"/>
       <c r="F15" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -4303,7 +4845,7 @@
       <c r="D16" s="18"/>
       <c r="E16" s="17"/>
       <c r="F16" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4315,7 +4857,7 @@
       <c r="D17" s="18"/>
       <c r="E17" s="17"/>
       <c r="F17" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4327,7 +4869,7 @@
       <c r="D18" s="18"/>
       <c r="E18" s="17"/>
       <c r="F18" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4339,7 +4881,7 @@
       <c r="D19" s="18"/>
       <c r="E19" s="17"/>
       <c r="F19" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4437,7 +4979,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4583,7 +5125,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4595,7 +5137,7 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4607,7 +5149,7 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4619,7 +5161,7 @@
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>